<commit_message>
change the exel file
</commit_message>
<xml_diff>
--- a/coffe_consumption.xlsx
+++ b/coffe_consumption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\dsa210project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63112EDE-9745-46F6-999F-0D177EC6AB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A4B942-EA73-4D65-A553-715E690C21AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E17D4BC5-2FD1-4A85-AF49-5CFB1261E235}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{E17D4BC5-2FD1-4A85-AF49-5CFB1261E235}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -431,9 +431,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F30EF4-2C64-452D-935B-8D7E290CC9F7}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1660,172 +1662,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>45992</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>45993</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>45994</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>45995</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>45996</v>
-      </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>45997</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>45998</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>45999</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>46000</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>46001</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>46002</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>46003</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>46004</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>46005</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
-        <v>46006</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>46007</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
-        <v>46008</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
-        <v>46009</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
-        <v>46010</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
-        <v>46011</v>
-      </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004E8E4F7D5234A74C92EAE85976469BDE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f5bd0eb488bd9db55dd8210ac2a2b6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6f083dfe-3067-48c6-831c-273595fb9351" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f8815efea909a2e7287477b57fc8f97" ns3:_="">
     <xsd:import namespace="6f083dfe-3067-48c6-831c-273595fb9351"/>
@@ -1981,15 +1832,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1999,6 +1841,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EE0ADA-DE17-41EA-AADF-0CDB58763864}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D77E1BE-42B4-4AAB-9902-915A01FA9A24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2012,14 +1862,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EE0ADA-DE17-41EA-AADF-0CDB58763864}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>